<commit_message>
Add SQL validation queries and update Excel output in listChampsOptions.py
</commit_message>
<xml_diff>
--- a/biops3/ListChampsOptions.xlsx
+++ b/biops3/ListChampsOptions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>NextStatusCode</t>
   </si>
@@ -28,6 +28,9 @@
     <t>OrderType</t>
   </si>
   <si>
+    <t>COLEDG_LedgType</t>
+  </si>
+  <si>
     <t>230</t>
   </si>
   <si>
@@ -130,16 +133,97 @@
     <t>09028</t>
   </si>
   <si>
+    <t>00072</t>
+  </si>
+  <si>
     <t>09015</t>
   </si>
   <si>
-    <t>00072</t>
-  </si>
-  <si>
     <t>OP</t>
   </si>
   <si>
     <t>ON</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>05</t>
   </si>
 </sst>
 </file>
@@ -497,13 +581,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,163 +600,257 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5">
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5">
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5">
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5">
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5">
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5">
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5">
+      <c r="C23" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="C15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3">
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3">
-      <c r="C18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3">
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3">
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3">
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3">
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3">
-      <c r="C23" t="s">
-        <v>39</v>
+      <c r="E23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5">
+      <c r="E24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5">
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5">
+      <c r="E26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5">
+      <c r="E27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5">
+      <c r="E28" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>